<commit_message>
updated queue name on config file
</commit_message>
<xml_diff>
--- a/AtRiskAssessmentPerformer/Data/Config.xlsx
+++ b/AtRiskAssessmentPerformer/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\P3\run-at-risk-assessment\AtRiskAssessmentPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96E3084-FA28-4297-8954-9CD085520CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11422" yWindow="1673" windowWidth="19800" windowHeight="14002" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -90,10 +90,6 @@
     <t>Framework</t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -122,6 +118,9 @@
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>AtRiskAssessmentQueue</t>
   </si>
 </sst>
 </file>
@@ -499,16 +498,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.59765625" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.3984375" customWidth="1"/>
+    <col min="4" max="26" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -547,17 +546,17 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="28.5">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -565,7 +564,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1574,12 +1573,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.3984375" customWidth="1"/>
+    <col min="4" max="26" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1616,7 +1615,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1624,7 +1623,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1648,7 +1647,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1670,7 +1669,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1681,7 +1680,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1692,7 +1691,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2682,16 +2681,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.86328125" customWidth="1"/>
+    <col min="2" max="2" width="30.1328125" customWidth="1"/>
+    <col min="3" max="3" width="60.265625" customWidth="1"/>
+    <col min="4" max="26" width="65.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2702,7 +2701,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Add workflow to generate an at-risk report for an associate
</commit_message>
<xml_diff>
--- a/AtRiskAssessmentPerformer/Data/Config.xlsx
+++ b/AtRiskAssessmentPerformer/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\P3\run-at-risk-assessment\AtRiskAssessmentPerformer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Revature\Revature-Capstone-1362\run-at-risk-assessment\AtRiskAssessmentPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96E3084-FA28-4297-8954-9CD085520CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1E4FE5-ECE4-451E-89DE-3FF15958520D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11422" yWindow="1673" windowWidth="19800" windowHeight="14002" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23370" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -121,6 +121,18 @@
   </si>
   <si>
     <t>AtRiskAssessmentQueue</t>
+  </si>
+  <si>
+    <t>OutputAssociateReportPath</t>
+  </si>
+  <si>
+    <t>OutputCohortReportPath</t>
+  </si>
+  <si>
+    <t>Path to directory for generated cohort reports.</t>
+  </si>
+  <si>
+    <t>Path to directory for generated associate reports.</t>
   </si>
 </sst>
 </file>
@@ -496,18 +508,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.59765625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.3984375" customWidth="1"/>
-    <col min="4" max="26" width="8.73046875" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -555,19 +567,33 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="28.5">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="30">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1560,6 +1586,7 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1573,12 +1600,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.3984375" customWidth="1"/>
-    <col min="4" max="26" width="8.73046875" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1615,7 +1642,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.5">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2685,12 +2712,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.86328125" customWidth="1"/>
-    <col min="2" max="2" width="30.1328125" customWidth="1"/>
-    <col min="3" max="3" width="60.265625" customWidth="1"/>
-    <col min="4" max="26" width="65.3984375" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Allow setting custom output directory and clean up project
</commit_message>
<xml_diff>
--- a/AtRiskAssessmentPerformer/Data/Config.xlsx
+++ b/AtRiskAssessmentPerformer/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\P3\run-at-risk-assessment\AtRiskAssessmentPerformer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Revature\Revature-Capstone-1362\run-at-risk-assessment\AtRiskAssessmentPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96E3084-FA28-4297-8954-9CD085520CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1E4FE5-ECE4-451E-89DE-3FF15958520D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11422" yWindow="1673" windowWidth="19800" windowHeight="14002" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23370" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -121,6 +121,18 @@
   </si>
   <si>
     <t>AtRiskAssessmentQueue</t>
+  </si>
+  <si>
+    <t>OutputAssociateReportPath</t>
+  </si>
+  <si>
+    <t>OutputCohortReportPath</t>
+  </si>
+  <si>
+    <t>Path to directory for generated cohort reports.</t>
+  </si>
+  <si>
+    <t>Path to directory for generated associate reports.</t>
   </si>
 </sst>
 </file>
@@ -496,18 +508,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.59765625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.3984375" customWidth="1"/>
-    <col min="4" max="26" width="8.73046875" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -555,19 +567,33 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="28.5">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="30">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1560,6 +1586,7 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1573,12 +1600,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.3984375" customWidth="1"/>
-    <col min="4" max="26" width="8.73046875" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1615,7 +1642,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.5">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2685,12 +2712,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.86328125" customWidth="1"/>
-    <col min="2" max="2" width="30.1328125" customWidth="1"/>
-    <col min="3" max="3" width="60.265625" customWidth="1"/>
-    <col min="4" max="26" width="65.3984375" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Add Trello API assets to config and start building workflow to get checklist completion
</commit_message>
<xml_diff>
--- a/AtRiskAssessmentPerformer/Data/Config.xlsx
+++ b/AtRiskAssessmentPerformer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Revature\Revature-Capstone-1362\run-at-risk-assessment\AtRiskAssessmentPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B6CF36-C64B-4ECF-9F4E-F891861A2D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47AF1F8-9241-4ABA-8774-147200BC9EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -175,6 +175,33 @@
   </si>
   <si>
     <t>P3 Automation</t>
+  </si>
+  <si>
+    <t>TrelloWorkspace</t>
+  </si>
+  <si>
+    <t>Id of Trello workspace containing cohort boards.</t>
+  </si>
+  <si>
+    <t>userworkspace95961868</t>
+  </si>
+  <si>
+    <t>TrelloAPIKey</t>
+  </si>
+  <si>
+    <t>TrelloAPISecret</t>
+  </si>
+  <si>
+    <t>Trello API Key</t>
+  </si>
+  <si>
+    <t>Trello API Secret</t>
+  </si>
+  <si>
+    <t>Oauth 1 secret for Trello API.</t>
+  </si>
+  <si>
+    <t>Developer key for Trello API.</t>
   </si>
 </sst>
 </file>
@@ -551,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1003"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -628,71 +655,81 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="5">
-        <v>465</v>
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="5">
+        <v>465</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
         <v>38</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>36</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="30">
-      <c r="A10" t="s">
+    <row r="11" spans="1:26" ht="30">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1685,6 +1722,7 @@
     <row r="1001" ht="14.25" customHeight="1"/>
     <row r="1002" ht="14.25" customHeight="1"/>
     <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2806,8 +2844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2854,8 +2892,34 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Complete workflow and associated changes to get Trello checklist completion when performing at-risk assessment
</commit_message>
<xml_diff>
--- a/AtRiskAssessmentPerformer/Data/Config.xlsx
+++ b/AtRiskAssessmentPerformer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Revature\Revature-Capstone-1362\run-at-risk-assessment\AtRiskAssessmentPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47AF1F8-9241-4ABA-8774-147200BC9EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3E1A11-D4C8-4FD6-9C82-386CE1F845D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,19 +189,19 @@
     <t>TrelloAPIKey</t>
   </si>
   <si>
-    <t>TrelloAPISecret</t>
-  </si>
-  <si>
     <t>Trello API Key</t>
   </si>
   <si>
-    <t>Trello API Secret</t>
-  </si>
-  <si>
-    <t>Oauth 1 secret for Trello API.</t>
-  </si>
-  <si>
-    <t>Developer key for Trello API.</t>
+    <t>TrelloAPIToken</t>
+  </si>
+  <si>
+    <t>Trello API Token</t>
+  </si>
+  <si>
+    <t>Token for Trello API.</t>
+  </si>
+  <si>
+    <t>Key for Trello API.</t>
   </si>
 </sst>
 </file>
@@ -2845,7 +2845,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2897,7 +2897,7 @@
         <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
         <v>49</v>
@@ -2908,7 +2908,7 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
         <v>56</v>

</xml_diff>